<commit_message>
Made a test change to the file
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Emily/Hunt-Exercises/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{92919507-5597-4A45-A468-DB40D5DD3699}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D220158-30E8-5141-9DFC-FB3A0EDEBF28}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14840" xr2:uid="{B2FFC057-19A9-524C-99D8-C004FC48A990}"/>
   </bookViews>
@@ -28,6 +28,14 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>Test change</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -377,12 +385,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41FD9919-64B7-244A-BD45-D9D40F2B41BA}">
-  <dimension ref="A1"/>
+  <dimension ref="B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>